<commit_message>
update README - maps viz
</commit_message>
<xml_diff>
--- a/MAPPING-COLS-ERD.xlsx
+++ b/MAPPING-COLS-ERD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal_project\REPO-SAA23\ecommerce-business-insight-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8AA40A-9182-4365-B1C2-6DB1CA93B495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C50FC9-381C-49BB-96C9-417A0A6AF8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="73" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76:C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,10 +958,6 @@
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C35" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">olist_order_reviews_dataset </v>
-      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1063,10 +1059,6 @@
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C45" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">olist_orders_dataset </v>
-      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -1180,10 +1172,6 @@
       <c r="A56" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C56" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">olist_products_dataset </v>
-      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -1309,10 +1297,6 @@
       <c r="A68" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C68" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">olist_sellers_dataset </v>
-      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
@@ -1377,10 +1361,6 @@
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C75" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">product_category_name_translation </v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>